<commit_message>
인터페이스 (parkinglot - server), 설계 문서 보완
</commit_message>
<xml_diff>
--- a/DesignDocuments/(5Team) Interface ParkingLot ↔ ParkServer.xlsx
+++ b/DesignDocuments/(5Team) Interface ParkingLot ↔ ParkServer.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sanghee3.lee\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\surepark\SureParkSystem\DesignDocuments\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="1200" yWindow="30" windowWidth="21555" windowHeight="10305" firstSheet="1" activeTab="1"/>
+    <workbookView xWindow="2160" yWindow="30" windowWidth="21555" windowHeight="10305" firstSheet="1" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Event Message" sheetId="2" state="hidden" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="117" uniqueCount="63">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="123" uniqueCount="68">
   <si>
     <t>DriverArriveAtExitGate</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -167,19 +167,11 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>slot_number (int)</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>id (string)
 pwd (string)</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>1~10</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>Parkingslot_LED</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -278,6 +270,51 @@
   <si>
     <t xml:space="preserve">ok or nok
 </t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>sensor_number (int)
+status (string)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>slot_number (int)
+slot_status (string[])
+led_status (string[])
+entrygate_status (string)
+exitgate_status (string)
+entrygateled_status (string)
+exitgateled_status (string)
+entrygate_arrive (string)
+exitgate_arrive (string)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>1~10
+empty or occupied
+on or off
+up or down
+up or down
+on or off
+on or off
+yes or no
+yes or no</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>HeartBeat</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>timestamp (int)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Acknowedge</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>-</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -957,10 +994,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B2:E24"/>
+  <dimension ref="B2:E26"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E11" sqref="E11"/>
+      <selection activeCell="D5" sqref="D5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -1001,24 +1038,24 @@
         <v>31</v>
       </c>
       <c r="D4" s="8" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="E4" s="1" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="5" spans="2:5" ht="33" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="2:5" ht="165" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B5" s="1">
         <v>2</v>
       </c>
       <c r="C5" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="D5" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="E5" s="1" t="s">
-        <v>38</v>
+      <c r="D5" s="8" t="s">
+        <v>62</v>
+      </c>
+      <c r="E5" s="8" t="s">
+        <v>63</v>
       </c>
     </row>
     <row r="6" spans="2:5" ht="33" customHeight="1" x14ac:dyDescent="0.3">
@@ -1026,13 +1063,13 @@
         <v>3</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="D6" s="8" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="E6" s="8" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
     </row>
     <row r="7" spans="2:5" ht="33" customHeight="1" x14ac:dyDescent="0.3">
@@ -1040,13 +1077,13 @@
         <v>4</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="D7" s="8" t="s">
+        <v>61</v>
+      </c>
+      <c r="E7" s="8" t="s">
         <v>57</v>
-      </c>
-      <c r="E7" s="8" t="s">
-        <v>59</v>
       </c>
     </row>
     <row r="8" spans="2:5" ht="33" customHeight="1" x14ac:dyDescent="0.3">
@@ -1054,13 +1091,13 @@
         <v>5</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="D8" s="8" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="E8" s="1" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
     </row>
     <row r="9" spans="2:5" ht="33" customHeight="1" x14ac:dyDescent="0.3">
@@ -1068,13 +1105,13 @@
         <v>6</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="D9" s="8" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="E9" s="1" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
     </row>
     <row r="10" spans="2:5" ht="33" customHeight="1" x14ac:dyDescent="0.3">
@@ -1082,13 +1119,13 @@
         <v>7</v>
       </c>
       <c r="C10" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="D10" s="8" t="s">
+        <v>39</v>
+      </c>
+      <c r="E10" s="1" t="s">
         <v>40</v>
-      </c>
-      <c r="D10" s="8" t="s">
-        <v>41</v>
-      </c>
-      <c r="E10" s="1" t="s">
-        <v>42</v>
       </c>
     </row>
     <row r="11" spans="2:5" ht="33" customHeight="1" x14ac:dyDescent="0.3">
@@ -1096,13 +1133,13 @@
         <v>8</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="D11" s="8" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="E11" s="1" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
     </row>
     <row r="12" spans="2:5" ht="33" customHeight="1" x14ac:dyDescent="0.3">
@@ -1110,13 +1147,13 @@
         <v>9</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="D12" s="8" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="E12" s="1" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
     </row>
     <row r="13" spans="2:5" ht="33" customHeight="1" x14ac:dyDescent="0.3">
@@ -1124,13 +1161,13 @@
         <v>10</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="D13" s="8" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="E13" s="1" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
     </row>
     <row r="14" spans="2:5" ht="33" customHeight="1" x14ac:dyDescent="0.3">
@@ -1138,13 +1175,13 @@
         <v>11</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="D14" s="8" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="E14" s="1" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
     </row>
     <row r="15" spans="2:5" ht="33" customHeight="1" x14ac:dyDescent="0.3">
@@ -1152,124 +1189,152 @@
         <v>12</v>
       </c>
       <c r="C15" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="D15" s="8" t="s">
+        <v>42</v>
+      </c>
+      <c r="E15" s="1" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="16" spans="2:5" ht="33" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B16" s="1">
+        <v>13</v>
+      </c>
+      <c r="C16" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="D16" s="8" t="s">
+        <v>65</v>
+      </c>
+      <c r="E16" s="1" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="18" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="C18" s="10" t="s">
         <v>50</v>
       </c>
-      <c r="D15" s="8" t="s">
-        <v>44</v>
-      </c>
-      <c r="E15" s="1" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="17" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="C17" s="10" t="s">
-        <v>52</v>
-      </c>
-      <c r="D17" s="10"/>
-      <c r="E17" s="10"/>
-    </row>
-    <row r="18" spans="2:5" ht="33" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B18" s="9" t="s">
+      <c r="D18" s="10"/>
+      <c r="E18" s="10"/>
+    </row>
+    <row r="19" spans="2:5" ht="33" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B19" s="9" t="s">
         <v>2</v>
       </c>
-      <c r="C18" s="9" t="s">
+      <c r="C19" s="9" t="s">
         <v>32</v>
       </c>
-      <c r="D18" s="9" t="s">
+      <c r="D19" s="9" t="s">
         <v>3</v>
       </c>
-      <c r="E18" s="9" t="s">
+      <c r="E19" s="9" t="s">
         <v>33</v>
-      </c>
-    </row>
-    <row r="19" spans="2:5" ht="33" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B19" s="1">
-        <v>1</v>
-      </c>
-      <c r="C19" s="1" t="s">
-        <v>53</v>
-      </c>
-      <c r="D19" s="8" t="s">
-        <v>61</v>
-      </c>
-      <c r="E19" s="8" t="s">
-        <v>62</v>
       </c>
     </row>
     <row r="20" spans="2:5" ht="33" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B20" s="1">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C20" s="1" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="D20" s="8" t="s">
-        <v>56</v>
-      </c>
-      <c r="E20" s="1" t="s">
-        <v>58</v>
+        <v>59</v>
+      </c>
+      <c r="E20" s="8" t="s">
+        <v>60</v>
       </c>
     </row>
     <row r="21" spans="2:5" ht="33" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B21" s="1">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C21" s="1" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="D21" s="8" t="s">
+        <v>54</v>
+      </c>
+      <c r="E21" s="1" t="s">
         <v>56</v>
-      </c>
-      <c r="E21" s="1" t="s">
-        <v>58</v>
       </c>
     </row>
     <row r="22" spans="2:5" ht="33" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B22" s="1">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C22" s="1" t="s">
-        <v>40</v>
+        <v>53</v>
       </c>
       <c r="D22" s="8" t="s">
+        <v>54</v>
+      </c>
+      <c r="E22" s="1" t="s">
         <v>56</v>
-      </c>
-      <c r="E22" s="1" t="s">
-        <v>42</v>
       </c>
     </row>
     <row r="23" spans="2:5" ht="33" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B23" s="1">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C23" s="1" t="s">
-        <v>43</v>
+        <v>38</v>
       </c>
       <c r="D23" s="8" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="E23" s="1" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
     </row>
     <row r="24" spans="2:5" ht="33" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B24" s="1">
+        <v>5</v>
+      </c>
+      <c r="C24" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="D24" s="8" t="s">
+        <v>54</v>
+      </c>
+      <c r="E24" s="1" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="25" spans="2:5" ht="33" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B25" s="1">
         <v>6</v>
       </c>
-      <c r="C24" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="D24" s="8" t="s">
+      <c r="C25" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="D25" s="8" t="s">
+        <v>55</v>
+      </c>
+      <c r="E25" s="8" t="s">
         <v>57</v>
       </c>
-      <c r="E24" s="8" t="s">
-        <v>59</v>
+    </row>
+    <row r="26" spans="2:5" ht="33" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B26" s="1">
+        <v>7</v>
+      </c>
+      <c r="C26" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="D26" s="8" t="s">
+        <v>65</v>
+      </c>
+      <c r="E26" s="8" t="s">
+        <v>67</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="2">
     <mergeCell ref="C2:E2"/>
-    <mergeCell ref="C17:E17"/>
+    <mergeCell ref="C18:E18"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
인터페이스 (parkinglot - server) 보완
</commit_message>
<xml_diff>
--- a/DesignDocuments/(5Team) Interface ParkingLot ↔ ParkServer.xlsx
+++ b/DesignDocuments/(5Team) Interface ParkingLot ↔ ParkServer.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="2160" yWindow="30" windowWidth="21555" windowHeight="10305" firstSheet="1" activeTab="1"/>
+    <workbookView xWindow="3120" yWindow="30" windowWidth="21555" windowHeight="10305" firstSheet="1" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Event Message" sheetId="2" state="hidden" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="123" uniqueCount="68">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="123" uniqueCount="69">
   <si>
     <t>DriverArriveAtExitGate</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -310,11 +310,15 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>Acknowedge</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>-</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Key / Value</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Ack</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -996,8 +1000,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:E26"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D5" sqref="D5"/>
+    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="C27" sqref="C27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -1024,7 +1028,7 @@
         <v>32</v>
       </c>
       <c r="D3" s="9" t="s">
-        <v>3</v>
+        <v>67</v>
       </c>
       <c r="E3" s="9" t="s">
         <v>33</v>
@@ -1322,13 +1326,13 @@
         <v>7</v>
       </c>
       <c r="C26" s="1" t="s">
-        <v>66</v>
+        <v>68</v>
       </c>
       <c r="D26" s="8" t="s">
         <v>65</v>
       </c>
       <c r="E26" s="8" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
     </row>
   </sheetData>

</xml_diff>